<commit_message>
edit R function v6
</commit_message>
<xml_diff>
--- a/data/hour_per_cnt_bySub_70RH______.xlsx
+++ b/data/hour_per_cnt_bySub_70RH______.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\API2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A4BF1A-04A4-49B5-85CB-E1FA765FFD7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC90CEE-A3D2-4A23-949F-A27A87B3130D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="115">
   <si>
     <t>project_code</t>
   </si>
@@ -360,6 +360,14 @@
   </si>
   <si>
     <t>1PD05Z480001</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1PD048270001</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1PD046550001</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -736,10 +744,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BD52"/>
+  <dimension ref="A1:BD54"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G2" sqref="A2:BD52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -4379,6 +4388,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="54" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="S54">
+        <f>SUM(S2:S16)+S18+S22+S23+S32+S35</f>
+        <v>767.39999999999986</v>
+      </c>
+      <c r="T54">
+        <f>S54/13</f>
+        <v>59.030769230769224</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4390,8 +4409,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60708917-66F2-468E-A4BE-C8BF7F1ABC3D}">
   <dimension ref="A1:BD45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="A5:XFD5"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -5246,7 +5266,7 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
         <v>56</v>
@@ -5829,7 +5849,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>114</v>
       </c>
       <c r="C22" t="s">
         <v>56</v>

</xml_diff>